<commit_message>
new alg + refactoring
</commit_message>
<xml_diff>
--- a/docs/расчеты размера.xlsx
+++ b/docs/расчеты размера.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\admin\Documents\discords_discovery\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA503A39-503F-4F60-AC70-360F6284C37B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C7AAC0-1929-4D58-A377-CF7266D50204}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,12 +74,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -110,6 +116,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -393,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +748,135 @@
         <v>16.867239492</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>2299</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>128</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" ref="D13:D19" si="10">A13-C13+1</f>
+        <v>2172</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" ref="E13:E19" si="11">D13*D13</f>
+        <v>4717584</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" ref="F13:F19" si="12">C13*D13</f>
+        <v>278016</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" ref="G13:G19" si="13">(E13+F13)*B13/1000000000</f>
+        <v>1.9982400000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>16090</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
+        <v>128</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="10"/>
+        <v>15963</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="11"/>
+        <v>254817369</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="12"/>
+        <v>2043264</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="13"/>
+        <v>1.027442532</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>32186</v>
+      </c>
+      <c r="B15" s="7">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7">
+        <v>128</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="10"/>
+        <v>32059</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="11"/>
+        <v>1027779481</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="12"/>
+        <v>4103552</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="13"/>
+        <v>4.1275321319999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>60000</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7">
+        <v>128</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="10"/>
+        <v>59873</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="11"/>
+        <v>3584776129</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="12"/>
+        <v>7663744</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="13"/>
+        <v>14.369759492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>